<commit_message>
Limpeza & Feedback 1
Limpando o código e aplicando os feedbacks da reunião 4. Criação de gráifcos e analise de dados.
</commit_message>
<xml_diff>
--- a/estatistica_descritiva_diferencas.xlsx
+++ b/estatistica_descritiva_diferencas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Diferencas" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Diferencas_Absolutas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Diferencas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Diferencas_Absolutas" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Gráficos - Aplicação Feedback 1
Criando gráficos planejados na reunião passada
</commit_message>
<xml_diff>
--- a/estatistica_descritiva_diferencas.xlsx
+++ b/estatistica_descritiva_diferencas.xlsx
@@ -474,13 +474,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1662156862745071</v>
+        <v>-0.02821568627450709</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1335223529411698</v>
+        <v>0.004477647058830195</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1437367647058781</v>
+        <v>-0.005736764705878084</v>
       </c>
     </row>
     <row r="4">
@@ -506,13 +506,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.2007700000000341</v>
+        <v>-0.06277000000003408</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1921699999999191</v>
+        <v>-0.05416999999991912</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.1914299999999685</v>
+        <v>-0.05342999999996845</v>
       </c>
     </row>
     <row r="6">
@@ -522,13 +522,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.1771624999999517</v>
+        <v>-0.03916249999995169</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.1458150000000273</v>
+        <v>-0.007815000000027328</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1538099999999645</v>
+        <v>-0.01580999999996446</v>
       </c>
     </row>
     <row r="7">
@@ -538,13 +538,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.1679300000000126</v>
+        <v>-0.02993000000001256</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1307100000000219</v>
+        <v>0.007289999999978147</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.1428699999999594</v>
+        <v>-0.004869999999959407</v>
       </c>
     </row>
     <row r="8">
@@ -554,13 +554,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.1552275000000236</v>
+        <v>-0.0172275000000236</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.11552999999995</v>
+        <v>0.02247000000005006</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1348649999999907</v>
+        <v>0.003135000000009325</v>
       </c>
     </row>
     <row r="9">
@@ -570,13 +570,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.1231700000000728</v>
+        <v>0.01482999999992718</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.09229000000004817</v>
+        <v>0.04570999999995184</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.08797000000004118</v>
+        <v>0.05002999999995883</v>
       </c>
     </row>
   </sheetData>
@@ -638,13 +638,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1662156862745071</v>
+        <v>0.02872666666666189</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1335223529411698</v>
+        <v>0.01974058823528968</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1437367647058781</v>
+        <v>0.0134865686274393</v>
       </c>
     </row>
     <row r="4">
@@ -654,13 +654,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01531695078034002</v>
+        <v>0.01432565781900236</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02342361020852004</v>
+        <v>0.01324251477893625</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01696136466824009</v>
+        <v>0.01171476875234177</v>
       </c>
     </row>
     <row r="5">
@@ -670,13 +670,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1231700000000728</v>
+        <v>0.0008099999999212626</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09229000000004817</v>
+        <v>0.0003000000000047409</v>
       </c>
       <c r="D5" t="n">
-        <v>0.08797000000004118</v>
+        <v>0.0001299999999792023</v>
       </c>
     </row>
     <row r="6">
@@ -686,13 +686,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1552275000000236</v>
+        <v>0.0172275000000236</v>
       </c>
       <c r="C6" t="n">
-        <v>0.11552999999995</v>
+        <v>0.007604999999989093</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1348649999999907</v>
+        <v>0.004259999999936315</v>
       </c>
     </row>
     <row r="7">
@@ -702,13 +702,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1679300000000126</v>
+        <v>0.02993000000001256</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1307100000000219</v>
+        <v>0.01735499999995227</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1428699999999594</v>
+        <v>0.01014500000002272</v>
       </c>
     </row>
     <row r="8">
@@ -718,13 +718,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1771624999999517</v>
+        <v>0.03916249999995169</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1458150000000273</v>
+        <v>0.02915999999998509</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1538099999999645</v>
+        <v>0.0188424999999936</v>
       </c>
     </row>
     <row r="9">
@@ -734,13 +734,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2007700000000341</v>
+        <v>0.06277000000003408</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1921699999999191</v>
+        <v>0.05416999999991912</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1914299999999685</v>
+        <v>0.05342999999996845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>